<commit_message>
Modification de la base, Ajout du fichier word et pdf
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,15 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinto Katende\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pinto Katende\Downloads\Pierre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC686E5C-3AE9-4C7A-8E32-05F031F7B68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCBC662-0522-48A2-B344-2F290CD85C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Année1" sheetId="2" r:id="rId2"/>
+    <sheet name="Univariée" sheetId="3" r:id="rId3"/>
+    <sheet name="Pearson" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="116">
   <si>
     <t>annee</t>
   </si>
@@ -310,13 +313,79 @@
   </si>
   <si>
     <t>47,684,200,972</t>
+  </si>
+  <si>
+    <t>Années</t>
+  </si>
+  <si>
+    <t>Mois</t>
+  </si>
+  <si>
+    <t>Rec_douane</t>
+  </si>
+  <si>
+    <t>Rec_connexe</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>Pearson</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>CI95%</t>
+  </si>
+  <si>
+    <t>p-val</t>
+  </si>
+  <si>
+    <t>BF10</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>[0.04, 0.51]</t>
+  </si>
+  <si>
+    <t>0.022648</t>
+  </si>
+  <si>
+    <t>2.035</t>
+  </si>
+  <si>
+    <t>0.634204</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,16 +407,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -370,15 +458,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,4 +1650,397 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E55FD3A-5160-4484-BE71-7287FC68C46F}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="A1:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6">
+        <v>46951137555</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>47313934748</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6">
+        <v>50398861182</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
+        <v>58775911887</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6">
+        <v>58775911887</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6">
+        <v>68656726875</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6">
+        <v>67199882580</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6">
+        <v>91744270326</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6">
+        <v>81660584134</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="6">
+        <v>86950027364</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6">
+        <v>77933324364</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>2018</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6">
+        <v>77055520300</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9C7415-9610-444A-85EA-3BC228074431}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="10">
+        <v>60</v>
+      </c>
+      <c r="C2" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="15">
+        <v>32195820</v>
+      </c>
+      <c r="C3" s="15">
+        <v>8885980</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="15">
+        <v>10407960</v>
+      </c>
+      <c r="C4" s="15">
+        <v>3792656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="15">
+        <v>18780460</v>
+      </c>
+      <c r="C5" s="15">
+        <v>2099507</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="B6" s="15">
+        <v>26823690</v>
+      </c>
+      <c r="C6" s="15">
+        <v>7049884</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="15">
+        <v>30515390</v>
+      </c>
+      <c r="C7" s="15">
+        <v>7949944</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="B8" s="15">
+        <v>34949840</v>
+      </c>
+      <c r="C8" s="15">
+        <v>9642040</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="15">
+        <v>88199660</v>
+      </c>
+      <c r="C9" s="15">
+        <v>19073680</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0.32329999999999998</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.42680000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F690BD-72E1-45B1-A24E-114DBEE5B33F}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="10">
+        <v>60</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.29389999999999999</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>